<commit_message>
Atualizado por script em 28-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/montenegro_prva-crnogorska-liga_2023-2024.xlsx
+++ b/2023/montenegro_prva-crnogorska-liga_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V84"/>
+  <dimension ref="A1:V85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5173,71 +5173,71 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Decic</t>
+          <t>Jezero</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Buducnost</t>
+          <t>Arsenal Tivat</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52" t="n">
-        <v>3.11</v>
+        <v>2.08</v>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>30/09/2023 12:43</t>
+          <t>30/09/2023 05:12</t>
         </is>
       </c>
       <c r="L52" t="n">
-        <v>2.82</v>
+        <v>2.41</v>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>01/10/2023 17:39</t>
+          <t>01/10/2023 17:50</t>
         </is>
       </c>
       <c r="N52" t="n">
-        <v>2.92</v>
+        <v>2.84</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>30/09/2023 12:43</t>
+          <t>30/09/2023 05:12</t>
         </is>
       </c>
       <c r="P52" t="n">
-        <v>2.79</v>
+        <v>2.84</v>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>01/10/2023 17:39</t>
+          <t>01/10/2023 17:50</t>
         </is>
       </c>
       <c r="R52" t="n">
-        <v>2.22</v>
+        <v>3.55</v>
       </c>
       <c r="S52" t="inlineStr">
         <is>
-          <t>30/09/2023 12:43</t>
+          <t>30/09/2023 05:12</t>
         </is>
       </c>
       <c r="T52" t="n">
-        <v>2.79</v>
+        <v>3.3</v>
       </c>
       <c r="U52" t="inlineStr">
         <is>
-          <t>01/10/2023 17:39</t>
+          <t>01/10/2023 17:50</t>
         </is>
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/montenegro/prva-crnogorska-liga/decic-buducnost/212AhUwR/</t>
+          <t>https://www.betexplorer.com/football/montenegro/prva-crnogorska-liga/jezero-arsenal-tivat/fya2fj9E/</t>
         </is>
       </c>
     </row>
@@ -5265,71 +5265,71 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Jezero</t>
+          <t>Sutjeska</t>
         </is>
       </c>
       <c r="G53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Arsenal Tivat</t>
+          <t>Mornar Bar</t>
         </is>
       </c>
       <c r="I53" t="n">
         <v>1</v>
       </c>
       <c r="J53" t="n">
-        <v>2.08</v>
+        <v>1.41</v>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>30/09/2023 05:12</t>
+          <t>01/10/2023 12:43</t>
         </is>
       </c>
       <c r="L53" t="n">
-        <v>2.41</v>
+        <v>1.51</v>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>01/10/2023 17:50</t>
+          <t>01/10/2023 17:46</t>
         </is>
       </c>
       <c r="N53" t="n">
-        <v>2.84</v>
+        <v>4.18</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>30/09/2023 05:12</t>
+          <t>01/10/2023 12:43</t>
         </is>
       </c>
       <c r="P53" t="n">
-        <v>2.84</v>
+        <v>3.88</v>
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>01/10/2023 17:50</t>
+          <t>01/10/2023 17:46</t>
         </is>
       </c>
       <c r="R53" t="n">
-        <v>3.55</v>
+        <v>7.18</v>
       </c>
       <c r="S53" t="inlineStr">
         <is>
-          <t>30/09/2023 05:12</t>
+          <t>01/10/2023 12:43</t>
         </is>
       </c>
       <c r="T53" t="n">
-        <v>3.3</v>
+        <v>6.55</v>
       </c>
       <c r="U53" t="inlineStr">
         <is>
-          <t>01/10/2023 17:50</t>
+          <t>01/10/2023 17:46</t>
         </is>
       </c>
       <c r="V53" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/montenegro/prva-crnogorska-liga/jezero-arsenal-tivat/fya2fj9E/</t>
+          <t>https://www.betexplorer.com/football/montenegro/prva-crnogorska-liga/sutjeska-mornar-bar/Gp0beWg8/</t>
         </is>
       </c>
     </row>
@@ -5357,71 +5357,71 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Sutjeska</t>
+          <t>Decic</t>
         </is>
       </c>
       <c r="G54" t="n">
+        <v>2</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Buducnost</t>
+        </is>
+      </c>
+      <c r="I54" t="n">
         <v>0</v>
       </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>Mornar Bar</t>
-        </is>
-      </c>
-      <c r="I54" t="n">
-        <v>1</v>
-      </c>
       <c r="J54" t="n">
-        <v>1.41</v>
+        <v>3.11</v>
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>01/10/2023 12:43</t>
+          <t>30/09/2023 12:43</t>
         </is>
       </c>
       <c r="L54" t="n">
-        <v>1.51</v>
+        <v>2.82</v>
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>01/10/2023 17:46</t>
+          <t>01/10/2023 17:39</t>
         </is>
       </c>
       <c r="N54" t="n">
-        <v>4.18</v>
+        <v>2.92</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>01/10/2023 12:43</t>
+          <t>30/09/2023 12:43</t>
         </is>
       </c>
       <c r="P54" t="n">
-        <v>3.88</v>
+        <v>2.79</v>
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>01/10/2023 17:46</t>
+          <t>01/10/2023 17:39</t>
         </is>
       </c>
       <c r="R54" t="n">
-        <v>7.18</v>
+        <v>2.22</v>
       </c>
       <c r="S54" t="inlineStr">
         <is>
-          <t>01/10/2023 12:43</t>
+          <t>30/09/2023 12:43</t>
         </is>
       </c>
       <c r="T54" t="n">
-        <v>6.55</v>
+        <v>2.79</v>
       </c>
       <c r="U54" t="inlineStr">
         <is>
-          <t>01/10/2023 17:46</t>
+          <t>01/10/2023 17:39</t>
         </is>
       </c>
       <c r="V54" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/montenegro/prva-crnogorska-liga/sutjeska-mornar-bar/Gp0beWg8/</t>
+          <t>https://www.betexplorer.com/football/montenegro/prva-crnogorska-liga/decic-buducnost/212AhUwR/</t>
         </is>
       </c>
     </row>
@@ -6093,7 +6093,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Sutjeska</t>
+          <t>Arsenal Tivat</t>
         </is>
       </c>
       <c r="G62" t="n">
@@ -6101,14 +6101,14 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Jedinstvo</t>
+          <t>Mornar Bar</t>
         </is>
       </c>
       <c r="I62" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J62" t="n">
-        <v>1.29</v>
+        <v>2.29</v>
       </c>
       <c r="K62" t="inlineStr">
         <is>
@@ -6116,15 +6116,15 @@
         </is>
       </c>
       <c r="L62" t="n">
-        <v>1.42</v>
+        <v>2.72</v>
       </c>
       <c r="M62" t="inlineStr">
         <is>
-          <t>21/10/2023 14:58</t>
+          <t>21/10/2023 14:43</t>
         </is>
       </c>
       <c r="N62" t="n">
-        <v>4.78</v>
+        <v>2.75</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -6132,15 +6132,15 @@
         </is>
       </c>
       <c r="P62" t="n">
-        <v>4.4</v>
+        <v>2.49</v>
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>21/10/2023 14:58</t>
+          <t>21/10/2023 14:43</t>
         </is>
       </c>
       <c r="R62" t="n">
-        <v>7.52</v>
+        <v>3.2</v>
       </c>
       <c r="S62" t="inlineStr">
         <is>
@@ -6148,16 +6148,16 @@
         </is>
       </c>
       <c r="T62" t="n">
-        <v>7.13</v>
+        <v>3.32</v>
       </c>
       <c r="U62" t="inlineStr">
         <is>
-          <t>21/10/2023 14:58</t>
+          <t>21/10/2023 14:43</t>
         </is>
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/montenegro/prva-crnogorska-liga/sutjeska-jedinstvo/MBIq7ThK/</t>
+          <t>https://www.betexplorer.com/football/montenegro/prva-crnogorska-liga/arsenal-tivat-mornar-bar/rLJu89wE/</t>
         </is>
       </c>
     </row>
@@ -6185,7 +6185,7 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Arsenal Tivat</t>
+          <t>Sutjeska</t>
         </is>
       </c>
       <c r="G63" t="n">
@@ -6193,14 +6193,14 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Mornar Bar</t>
+          <t>Jedinstvo</t>
         </is>
       </c>
       <c r="I63" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J63" t="n">
-        <v>2.29</v>
+        <v>1.29</v>
       </c>
       <c r="K63" t="inlineStr">
         <is>
@@ -6208,15 +6208,15 @@
         </is>
       </c>
       <c r="L63" t="n">
-        <v>2.72</v>
+        <v>1.42</v>
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>21/10/2023 14:43</t>
+          <t>21/10/2023 14:58</t>
         </is>
       </c>
       <c r="N63" t="n">
-        <v>2.75</v>
+        <v>4.78</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -6224,15 +6224,15 @@
         </is>
       </c>
       <c r="P63" t="n">
-        <v>2.49</v>
+        <v>4.4</v>
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>21/10/2023 14:43</t>
+          <t>21/10/2023 14:58</t>
         </is>
       </c>
       <c r="R63" t="n">
-        <v>3.2</v>
+        <v>7.52</v>
       </c>
       <c r="S63" t="inlineStr">
         <is>
@@ -6240,16 +6240,16 @@
         </is>
       </c>
       <c r="T63" t="n">
-        <v>3.32</v>
+        <v>7.13</v>
       </c>
       <c r="U63" t="inlineStr">
         <is>
-          <t>21/10/2023 14:43</t>
+          <t>21/10/2023 14:58</t>
         </is>
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/montenegro/prva-crnogorska-liga/arsenal-tivat-mornar-bar/rLJu89wE/</t>
+          <t>https://www.betexplorer.com/football/montenegro/prva-crnogorska-liga/sutjeska-jedinstvo/MBIq7ThK/</t>
         </is>
       </c>
     </row>
@@ -7013,22 +7013,22 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Rudar</t>
+          <t>Arsenal Tivat</t>
         </is>
       </c>
       <c r="G72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Decic</t>
+          <t>Buducnost</t>
         </is>
       </c>
       <c r="I72" t="n">
         <v>1</v>
       </c>
       <c r="J72" t="n">
-        <v>4.05</v>
+        <v>4.24</v>
       </c>
       <c r="K72" t="inlineStr">
         <is>
@@ -7036,15 +7036,15 @@
         </is>
       </c>
       <c r="L72" t="n">
-        <v>3.94</v>
+        <v>5.09</v>
       </c>
       <c r="M72" t="inlineStr">
         <is>
-          <t>05/11/2023 13:24</t>
+          <t>05/11/2023 06:36</t>
         </is>
       </c>
       <c r="N72" t="n">
-        <v>3.2</v>
+        <v>3.29</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -7052,15 +7052,15 @@
         </is>
       </c>
       <c r="P72" t="n">
-        <v>3.06</v>
+        <v>3.75</v>
       </c>
       <c r="Q72" t="inlineStr">
         <is>
-          <t>05/11/2023 13:24</t>
+          <t>05/11/2023 06:36</t>
         </is>
       </c>
       <c r="R72" t="n">
-        <v>1.8</v>
+        <v>1.74</v>
       </c>
       <c r="S72" t="inlineStr">
         <is>
@@ -7068,16 +7068,16 @@
         </is>
       </c>
       <c r="T72" t="n">
-        <v>2.04</v>
+        <v>1.63</v>
       </c>
       <c r="U72" t="inlineStr">
         <is>
-          <t>05/11/2023 13:11</t>
+          <t>05/11/2023 06:36</t>
         </is>
       </c>
       <c r="V72" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/montenegro/prva-crnogorska-liga/rudar-decic/UkVe0Iy5/</t>
+          <t>https://www.betexplorer.com/football/montenegro/prva-crnogorska-liga/arsenal-tivat-buducnost/GQFj3Kin/</t>
         </is>
       </c>
     </row>
@@ -7105,22 +7105,22 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Arsenal Tivat</t>
+          <t>Rudar</t>
         </is>
       </c>
       <c r="G73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Buducnost</t>
+          <t>Decic</t>
         </is>
       </c>
       <c r="I73" t="n">
         <v>1</v>
       </c>
       <c r="J73" t="n">
-        <v>4.24</v>
+        <v>4.05</v>
       </c>
       <c r="K73" t="inlineStr">
         <is>
@@ -7128,15 +7128,15 @@
         </is>
       </c>
       <c r="L73" t="n">
-        <v>5.09</v>
+        <v>3.94</v>
       </c>
       <c r="M73" t="inlineStr">
         <is>
-          <t>05/11/2023 06:36</t>
+          <t>05/11/2023 13:24</t>
         </is>
       </c>
       <c r="N73" t="n">
-        <v>3.29</v>
+        <v>3.2</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
@@ -7144,15 +7144,15 @@
         </is>
       </c>
       <c r="P73" t="n">
-        <v>3.75</v>
+        <v>3.06</v>
       </c>
       <c r="Q73" t="inlineStr">
         <is>
-          <t>05/11/2023 06:36</t>
+          <t>05/11/2023 13:24</t>
         </is>
       </c>
       <c r="R73" t="n">
-        <v>1.74</v>
+        <v>1.8</v>
       </c>
       <c r="S73" t="inlineStr">
         <is>
@@ -7160,16 +7160,16 @@
         </is>
       </c>
       <c r="T73" t="n">
-        <v>1.63</v>
+        <v>2.04</v>
       </c>
       <c r="U73" t="inlineStr">
         <is>
-          <t>05/11/2023 06:36</t>
+          <t>05/11/2023 13:11</t>
         </is>
       </c>
       <c r="V73" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/montenegro/prva-crnogorska-liga/arsenal-tivat-buducnost/GQFj3Kin/</t>
+          <t>https://www.betexplorer.com/football/montenegro/prva-crnogorska-liga/rudar-decic/UkVe0Iy5/</t>
         </is>
       </c>
     </row>
@@ -8182,6 +8182,98 @@
       <c r="V84" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/montenegro/prva-crnogorska-liga/jezero-rudar/G6gwDeLA/</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>montenegro</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>prva-crnogorska-liga</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E85" s="2" t="n">
+        <v>45258.54166666666</v>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Jedinstvo</t>
+        </is>
+      </c>
+      <c r="G85" t="n">
+        <v>1</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Petrovac</t>
+        </is>
+      </c>
+      <c r="I85" t="n">
+        <v>1</v>
+      </c>
+      <c r="J85" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>24/11/2023 02:12</t>
+        </is>
+      </c>
+      <c r="L85" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>28/11/2023 12:46</t>
+        </is>
+      </c>
+      <c r="N85" t="n">
+        <v>2.91</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>24/11/2023 02:12</t>
+        </is>
+      </c>
+      <c r="P85" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="Q85" t="inlineStr">
+        <is>
+          <t>28/11/2023 11:12</t>
+        </is>
+      </c>
+      <c r="R85" t="n">
+        <v>2.54</v>
+      </c>
+      <c r="S85" t="inlineStr">
+        <is>
+          <t>24/11/2023 02:12</t>
+        </is>
+      </c>
+      <c r="T85" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="U85" t="inlineStr">
+        <is>
+          <t>28/11/2023 12:46</t>
+        </is>
+      </c>
+      <c r="V85" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/montenegro/prva-crnogorska-liga/jedinstvo-petrovac/Sp1QFcyh/</t>
         </is>
       </c>
     </row>

</xml_diff>